<commit_message>
Respuestas de observaciones lab-7
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49260205965f8aee/Documentos/Trabajos EDA/Lab7/LabCollision-S07-G08/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6E5986-5D76-40E6-8BB6-4E7550720C79}"/>
+  <xr:revisionPtr revIDLastSave="535" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F641D17C-5298-4B05-BFB2-53A18D6FA7D1}"/>
   <bookViews>
-    <workbookView xWindow="-2127" yWindow="7073" windowWidth="4267" windowHeight="2354" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="767" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -481,7 +481,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -568,7 +568,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -580,13 +580,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1729157.47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>1729157.52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>1729157.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -598,13 +598,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>43643.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>43395.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>45815.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,7 +694,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -706,13 +706,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1729179.81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>1729179.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140</c:v>
+                  <c:v>1729179.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -724,13 +724,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>47989.19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>45605.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>44752.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,7 +835,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -873,7 +873,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -957,7 +957,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -995,7 +995,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1037,7 +1037,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1074,7 +1074,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1637,7 +1637,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CA07E00A-1DDB-47A3-B681-B59870FF7EA9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1648,7 +1648,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8660296" cy="6281530"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1702,7 +1702,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2000,25 +2000,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.8203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2029,47 +2029,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.3</v>
       </c>
       <c r="B3" s="2">
-        <v>100</v>
+        <v>1729157.47</v>
       </c>
       <c r="C3" s="2">
-        <v>45</v>
+        <v>43643.18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.5</v>
       </c>
       <c r="B4" s="2">
-        <v>105</v>
+        <v>1729157.52</v>
       </c>
       <c r="C4" s="2">
-        <v>55</v>
+        <v>43395.05</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.8</v>
       </c>
       <c r="B5" s="2">
-        <v>115</v>
+        <v>1729157.58</v>
       </c>
       <c r="C5" s="2">
-        <v>75</v>
+        <v>45815.64</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2080,40 +2080,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2</v>
       </c>
       <c r="B10" s="2">
-        <v>100</v>
+        <v>1729179.81</v>
       </c>
       <c r="C10" s="2">
-        <v>90</v>
+        <v>47989.19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>4</v>
       </c>
       <c r="B11" s="2">
-        <v>120</v>
+        <v>1729179.83</v>
       </c>
       <c r="C11" s="2">
-        <v>100</v>
+        <v>45605.87</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>140</v>
+        <v>1729179.85</v>
       </c>
       <c r="C12" s="2">
-        <v>110</v>
+        <v>44752.82</v>
       </c>
     </row>
-    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>